<commit_message>
Adder - schematic tweak
</commit_message>
<xml_diff>
--- a/modules/Adder/Adder-BOM.xlsx
+++ b/modules/Adder/Adder-BOM.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Len\Documents\Dev\git\Synth-priv\modules\Adder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\git\Synth-priv\modules\Adder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B134F126-49FE-45D6-BE9A-8387C5662CF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00251E32-83EE-4B9E-B5A0-B864AD620A29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4080" yWindow="1695" windowWidth="19380" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Adder-BOM" sheetId="1" r:id="rId1"/>
@@ -1363,27 +1363,28 @@
   <dimension ref="A1:U17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <pane xSplit="6" topLeftCell="O1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="4.1328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="4.1328125" customWidth="1"/>
-    <col min="11" max="11" width="17.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="4.140625" customWidth="1"/>
+    <col min="11" max="11" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="21" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.59765625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="22.59765625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="145.1328125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.59765625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="28.265625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="107.86328125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.73046875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="19.73046875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="54.86328125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="145.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="107.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="54.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="1" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:21" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1448,7 +1449,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -1490,7 +1491,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -1529,7 +1530,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>156</v>
       </c>
@@ -1583,7 +1584,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>49</v>
       </c>
@@ -1625,7 +1626,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>58</v>
       </c>
@@ -1664,7 +1665,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>66</v>
       </c>
@@ -1721,7 +1722,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>78</v>
       </c>
@@ -1766,7 +1767,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>85</v>
       </c>
@@ -1805,7 +1806,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>91</v>
       </c>
@@ -1844,7 +1845,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>96</v>
       </c>
@@ -1886,7 +1887,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>105</v>
       </c>
@@ -1928,7 +1929,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>113</v>
       </c>
@@ -1973,7 +1974,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>120</v>
       </c>
@@ -2015,7 +2016,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>127</v>
       </c>
@@ -2051,7 +2052,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>136</v>
       </c>
@@ -2096,7 +2097,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>145</v>
       </c>

</xml_diff>

<commit_message>
Adder - BOM update
</commit_message>
<xml_diff>
--- a/modules/Adder/Adder-BOM.xlsx
+++ b/modules/Adder/Adder-BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\git\Synth-priv\modules\Adder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00251E32-83EE-4B9E-B5A0-B864AD620A29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A9BCA4B-0685-454B-B5D3-AB38702C0438}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4080" yWindow="1695" windowWidth="19380" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4155" yWindow="2325" windowWidth="19380" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Adder-BOM" sheetId="1" r:id="rId1"/>
@@ -1363,8 +1363,8 @@
   <dimension ref="A1:U17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="6" topLeftCell="O1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="O3" sqref="O3"/>
+      <pane xSplit="6" topLeftCell="G1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1498,9 +1498,12 @@
       <c r="B3">
         <v>2</v>
       </c>
+      <c r="D3">
+        <v>20</v>
+      </c>
       <c r="E3">
         <f t="shared" ref="E3:E17" si="0">MAX(0,B3-C3-D3)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F3" t="s">
         <v>29</v>
@@ -1897,9 +1900,12 @@
       <c r="C12">
         <v>4</v>
       </c>
+      <c r="D12">
+        <v>10</v>
+      </c>
       <c r="E12">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="F12" t="s">
         <v>106</v>
@@ -2023,9 +2029,12 @@
       <c r="B15">
         <v>2</v>
       </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
       <c r="E15">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F15" t="s">
         <v>128</v>
@@ -2059,9 +2068,12 @@
       <c r="B16">
         <v>1</v>
       </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
       <c r="E16">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F16" t="s">
         <v>137</v>

</xml_diff>